<commit_message>
Fixed a bug in yearfrac and vba in the naming of vba modules. RangeAddress worksheet is set to "" if null. Fixed some tests
</commit_message>
<xml_diff>
--- a/EPPlusTest/worksheets/copy.xlsx
+++ b/EPPlusTest/worksheets/copy.xlsx
@@ -36,6 +36,10 @@
     </font>
     <font>
       <sz val="11"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FFFF0000" tint="0"/>
       <name val="Calibri"/>
     </font>
@@ -44,10 +48,6 @@
       <sz val="11"/>
       <color rgb="FF0000FF" tint="0"/>
       <name val="Calibri"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <name val="Times New Roman"/>
     </font>
     <font>
       <sz val="11"/>
@@ -85,17 +85,18 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" xfId="0"/>
     <xf numFmtId="0" fontId="2" xfId="0"/>
+    <xf numFmtId="0" fontId="3" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="2" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="3" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="3" xfId="0"/>
     <xf numFmtId="164" fontId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="3" xfId="0"/>
-    <xf numFmtId="28" fontId="3" xfId="0"/>
+    <xf numFmtId="28" fontId="1" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -112,182 +113,185 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="9.140625" customWidth="1"/>
+    <col min="1" max="1" width="9.140625" customWidth="1"/>
+    <col min="2" max="2" width="9.140625" customWidth="1" style="1"/>
+    <col min="3" max="3" width="9.140625" customWidth="1"/>
+    <col min="7" max="7" width="9.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="G1" s="2" t="s">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="G1" s="3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" s="3" customFormat="1">
-      <c r="A2" s="4" t="s">
+    <row r="2" s="4" customFormat="1">
+      <c r="A2" s="5" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="G3" s="2" t="s">
+      <c r="A3" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="G3" s="3" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B4" s="6"/>
-      <c r="C4" s="7">
+      <c r="A4" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" s="7"/>
+      <c r="C4" s="8">
         <f ref="C4:G4" t="shared" si="1">B4+B$1</f>
       </c>
-      <c r="D4" s="7">
+      <c r="D4" s="8">
         <f t="shared" si="1"/>
       </c>
-      <c r="E4" s="7">
+      <c r="E4" s="8">
         <f t="shared" si="1"/>
       </c>
-      <c r="F4" s="7">
+      <c r="F4" s="8">
         <f t="shared" si="1"/>
       </c>
-      <c r="G4" s="7">
+      <c r="G4" s="8">
         <f t="shared" si="1"/>
       </c>
     </row>
     <row r="5">
-      <c r="B5" s="8" t="s">
+      <c r="B5" s="9" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="6">
-      <c r="B6" s="8" t="s">
+      <c r="B6" s="9" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="7">
-      <c r="B7" s="8" t="s">
+      <c r="B7" s="9" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="8">
-      <c r="B8" s="6"/>
-      <c r="H8" s="7">
+      <c r="B8" s="7"/>
+      <c r="H8" s="8">
         <f ref="H8:H30" t="shared" si="2">G8+G$1</f>
       </c>
     </row>
     <row r="9">
-      <c r="H9" s="7">
+      <c r="H9" s="8">
         <f t="shared" si="2"/>
       </c>
     </row>
     <row r="10">
-      <c r="H10" s="7">
+      <c r="H10" s="8">
         <f t="shared" si="2"/>
       </c>
     </row>
     <row r="11">
-      <c r="H11" s="7">
+      <c r="H11" s="8">
         <f t="shared" si="2"/>
       </c>
     </row>
     <row r="12">
-      <c r="H12" s="7">
+      <c r="H12" s="8">
         <f t="shared" si="2"/>
       </c>
     </row>
     <row r="13">
-      <c r="H13" s="7">
+      <c r="H13" s="8">
         <f t="shared" si="2"/>
       </c>
     </row>
     <row r="14">
-      <c r="H14" s="7">
+      <c r="H14" s="8">
         <f t="shared" si="2"/>
       </c>
     </row>
     <row r="15">
-      <c r="B15" s="9">
+      <c r="B15" s="10">
         <f>A15+A$1</f>
       </c>
-      <c r="H15" s="7">
+      <c r="H15" s="8">
         <f t="shared" si="2"/>
       </c>
     </row>
     <row r="16">
-      <c r="H16" s="7">
+      <c r="H16" s="8">
         <f t="shared" si="2"/>
       </c>
     </row>
     <row r="17">
-      <c r="H17" s="7">
+      <c r="H17" s="8">
         <f t="shared" si="2"/>
       </c>
     </row>
     <row r="18">
-      <c r="H18" s="7">
+      <c r="H18" s="8">
         <f t="shared" si="2"/>
       </c>
     </row>
     <row r="19">
-      <c r="H19" s="7">
+      <c r="H19" s="8">
         <f t="shared" si="2"/>
       </c>
     </row>
     <row r="20">
-      <c r="H20" s="7">
+      <c r="H20" s="8">
         <f t="shared" si="2"/>
       </c>
     </row>
     <row r="21">
-      <c r="H21" s="7">
+      <c r="H21" s="8">
         <f t="shared" si="2"/>
       </c>
     </row>
     <row r="22">
-      <c r="H22" s="7">
+      <c r="H22" s="8">
         <f t="shared" si="2"/>
       </c>
     </row>
     <row r="23">
-      <c r="H23" s="7">
+      <c r="H23" s="8">
         <f t="shared" si="2"/>
       </c>
     </row>
     <row r="24">
-      <c r="H24" s="7">
+      <c r="H24" s="8">
         <f t="shared" si="2"/>
       </c>
     </row>
     <row r="25">
-      <c r="H25" s="7">
+      <c r="H25" s="8">
         <f t="shared" si="2"/>
       </c>
     </row>
     <row r="26">
-      <c r="H26" s="7">
+      <c r="H26" s="8">
         <f t="shared" si="2"/>
       </c>
     </row>
     <row r="27">
-      <c r="H27" s="7">
+      <c r="H27" s="8">
         <f t="shared" si="2"/>
       </c>
     </row>
     <row r="28">
-      <c r="H28" s="7">
+      <c r="H28" s="8">
         <f t="shared" si="2"/>
       </c>
     </row>
     <row r="29">
-      <c r="H29" s="7">
+      <c r="H29" s="8">
         <f t="shared" si="2"/>
       </c>
     </row>
     <row r="30">
-      <c r="H30" s="7">
+      <c r="H30" s="8">
         <f t="shared" si="2"/>
       </c>
     </row>

</xml_diff>

<commit_message>
Final preparations for version 4.0 Beta. Fixed tests and a few bugs.
</commit_message>
<xml_diff>
--- a/EPPlusTest/worksheets/copy.xlsx
+++ b/EPPlusTest/worksheets/copy.xlsx
@@ -83,20 +83,20 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0"/>
+    <xf numFmtId="0" applyNumberFormat="1" fontId="0" applyFont="1"/>
   </cellStyleXfs>
   <cellXfs count="11">
-    <xf numFmtId="0" fontId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" xfId="0"/>
-    <xf numFmtId="0" fontId="2" xfId="0"/>
-    <xf numFmtId="0" fontId="3" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="2" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="3" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="3" xfId="0"/>
-    <xf numFmtId="164" fontId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="3" xfId="0"/>
-    <xf numFmtId="28" fontId="1" xfId="0"/>
+    <xf numFmtId="0" applyNumberFormat="1" fontId="0" applyFont="1" xfId="0"/>
+    <xf numFmtId="0" applyNumberFormat="1" fontId="1" applyFont="1" xfId="0"/>
+    <xf numFmtId="0" applyNumberFormat="1" fontId="2" applyFont="1" xfId="0"/>
+    <xf numFmtId="0" applyNumberFormat="1" fontId="3" applyFont="1" xfId="0"/>
+    <xf numFmtId="0" applyNumberFormat="1" fontId="0" applyFont="1" fillId="2" applyFill="1" xfId="0"/>
+    <xf numFmtId="0" applyNumberFormat="1" fontId="2" applyFont="1" fillId="2" applyFill="1" xfId="0"/>
+    <xf numFmtId="0" applyNumberFormat="1" fontId="2" applyFont="1" fillId="3" applyFill="1" xfId="0"/>
+    <xf numFmtId="0" applyNumberFormat="1" fontId="1" applyFont="1" fillId="3" applyFill="1" xfId="0"/>
+    <xf numFmtId="164" applyNumberFormat="1" fontId="0" applyFont="1" xfId="0"/>
+    <xf numFmtId="0" applyNumberFormat="1" fontId="4" applyFont="1" fillId="3" applyFill="1" xfId="0"/>
+    <xf numFmtId="28" applyNumberFormat="1" fontId="1" applyFont="1" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>

</xml_diff>